<commit_message>
Separate out the lat and lon in data file
</commit_message>
<xml_diff>
--- a/data/bad_postcode_data_Thev.xlsx
+++ b/data/bad_postcode_data_Thev.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiannmeng\src\mys-postcode-matrix\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E38B70-6331-4AC1-A396-EED32C027ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B21BE47-EF90-4E87-8A52-E8064C838594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18048" yWindow="1680" windowWidth="12288" windowHeight="3360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21504" yWindow="972" windowWidth="13344" windowHeight="12444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="33">
   <si>
     <t>postcode</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>(1.9569694921352196, 103.20613036639183)</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lon</t>
   </si>
 </sst>
 </file>
@@ -514,23 +520,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.44140625" customWidth="1"/>
+    <col min="6" max="6" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -547,8 +554,14 @@
       <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="6">
         <v>2799</v>
       </c>
@@ -567,8 +580,14 @@
       <c r="F2" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="7">
+        <v>6.3424724379990103</v>
+      </c>
+      <c r="H2" s="7">
+        <v>100.18982195228899</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="6">
         <v>3624</v>
       </c>
@@ -587,8 +606,14 @@
       <c r="F3" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="7">
+        <v>6.3424724379990103</v>
+      </c>
+      <c r="H3" s="7">
+        <v>100.18982195228899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="6">
         <v>3625</v>
       </c>
@@ -607,8 +632,14 @@
       <c r="F4" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="7">
+        <v>6.3424724379990103</v>
+      </c>
+      <c r="H4" s="7">
+        <v>100.18982195228899</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="6">
         <v>3626</v>
       </c>
@@ -627,8 +658,14 @@
       <c r="F5" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="7">
+        <v>6.3424724379990103</v>
+      </c>
+      <c r="H5" s="7">
+        <v>100.18982195228899</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="6">
         <v>600</v>
       </c>
@@ -647,8 +684,14 @@
       <c r="F6" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="7">
+        <v>5.2839549999999997</v>
+      </c>
+      <c r="H6" s="7">
+        <v>100.47694300000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="6">
         <v>1913</v>
       </c>
@@ -667,8 +710,14 @@
       <c r="F7" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="7">
+        <v>5.2839549999999997</v>
+      </c>
+      <c r="H7" s="7">
+        <v>100.47694300000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="6">
         <v>1921</v>
       </c>
@@ -687,8 +736,14 @@
       <c r="F8" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="7">
+        <v>5.2839549999999997</v>
+      </c>
+      <c r="H8" s="7">
+        <v>100.47694300000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="4">
         <v>6153</v>
       </c>
@@ -707,8 +762,14 @@
       <c r="F9" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="5">
+        <v>6.2167546897344304</v>
+      </c>
+      <c r="H9" s="5">
+        <v>100.39997806495001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="4">
         <v>7573</v>
       </c>
@@ -727,8 +788,14 @@
       <c r="F10" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="5">
+        <v>6.2167546897344304</v>
+      </c>
+      <c r="H10" s="5">
+        <v>100.39997806495001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="4">
         <v>7574</v>
       </c>
@@ -747,8 +814,14 @@
       <c r="F11" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="5">
+        <v>6.2167546897344304</v>
+      </c>
+      <c r="H11" s="5">
+        <v>100.39997806495001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="4">
         <v>641</v>
       </c>
@@ -767,8 +840,14 @@
       <c r="F12" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="5">
+        <v>5.2180408570779102</v>
+      </c>
+      <c r="H12" s="5">
+        <v>100.495090233852</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="4">
         <v>9673</v>
       </c>
@@ -787,8 +866,14 @@
       <c r="F13" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" s="5">
+        <v>5.2180408570779102</v>
+      </c>
+      <c r="H13" s="5">
+        <v>100.495090233852</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="4">
         <v>4372</v>
       </c>
@@ -807,8 +892,14 @@
       <c r="F14" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" s="5">
+        <v>5.2180408570779102</v>
+      </c>
+      <c r="H14" s="5">
+        <v>100.495090233852</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="6">
         <v>9333</v>
       </c>
@@ -827,8 +918,14 @@
       <c r="F15" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" s="7">
+        <v>5.6044875486454204</v>
+      </c>
+      <c r="H15" s="7">
+        <v>100.7721031256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="6">
         <v>68982</v>
       </c>
@@ -847,8 +944,14 @@
       <c r="F16" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="7">
+        <v>2.9305659999999998</v>
+      </c>
+      <c r="H16" s="7">
+        <v>112.542298</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="4">
         <v>6360</v>
       </c>
@@ -867,8 +970,14 @@
       <c r="F17" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" s="5">
+        <v>5.2121177699999999</v>
+      </c>
+      <c r="H17" s="5">
+        <v>100.61685221</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="4">
         <v>7358</v>
       </c>
@@ -887,8 +996,14 @@
       <c r="F18" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" s="5">
+        <v>5.2121177699999999</v>
+      </c>
+      <c r="H18" s="5">
+        <v>100.61685221</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="4">
         <v>8462</v>
       </c>
@@ -907,8 +1022,14 @@
       <c r="F19" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" s="5">
+        <v>5.2121177699999999</v>
+      </c>
+      <c r="H19" s="5">
+        <v>100.61685221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="4">
         <v>46504</v>
       </c>
@@ -927,8 +1048,14 @@
       <c r="F20" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" s="5">
+        <v>2.9925905249915501</v>
+      </c>
+      <c r="H20" s="5">
+        <v>101.7048806187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="6">
         <v>9711</v>
       </c>
@@ -947,8 +1074,14 @@
       <c r="F21" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21" s="7">
+        <v>6.0185647383898502</v>
+      </c>
+      <c r="H21" s="7">
+        <v>101.97637471265099</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="6">
         <v>7363</v>
       </c>
@@ -967,8 +1100,14 @@
       <c r="F22" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22" s="7">
+        <v>6.0185647383898502</v>
+      </c>
+      <c r="H22" s="7">
+        <v>101.97637471265099</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="6">
         <v>40300</v>
       </c>
@@ -987,8 +1126,14 @@
       <c r="F23" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" s="7">
+        <v>5.2410259999999997</v>
+      </c>
+      <c r="H23" s="7">
+        <v>100.73147400000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="4">
         <v>254</v>
       </c>
@@ -1007,8 +1152,14 @@
       <c r="F24" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" s="5">
+        <v>3.1003786899999999</v>
+      </c>
+      <c r="H24" s="5">
+        <v>101.80299706</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="4">
         <v>448</v>
       </c>
@@ -1027,8 +1178,14 @@
       <c r="F25" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25" s="5">
+        <v>3.2602378698699601</v>
+      </c>
+      <c r="H25" s="5">
+        <v>101.733398717619</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="6">
         <v>56852</v>
       </c>
@@ -1047,8 +1204,14 @@
       <c r="F26" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26" s="7">
+        <v>4.39372302058689</v>
+      </c>
+      <c r="H26" s="7">
+        <v>101.19221718279</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="6">
         <v>6140</v>
       </c>
@@ -1067,8 +1230,14 @@
       <c r="F27" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27" s="7">
+        <v>3.2609900000000001</v>
+      </c>
+      <c r="H27" s="7">
+        <v>101.30480799999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="4">
         <v>6029</v>
       </c>
@@ -1087,8 +1256,14 @@
       <c r="F28" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28" s="5">
+        <v>1.9569694921352101</v>
+      </c>
+      <c r="H28" s="5">
+        <v>103.20613036639099</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="4">
         <v>19789</v>
       </c>
@@ -1107,8 +1282,14 @@
       <c r="F29" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29" s="5">
+        <v>1.9569694921352101</v>
+      </c>
+      <c r="H29" s="5">
+        <v>103.20613036639099</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="4">
         <v>6891</v>
       </c>
@@ -1127,11 +1308,17 @@
       <c r="F30" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30" s="5">
+        <v>6.2382590000000002</v>
+      </c>
+      <c r="H30" s="5">
+        <v>100.245701</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:8">
       <c r="A32" s="2"/>
     </row>
   </sheetData>

</xml_diff>